<commit_message>
batarya ve esc değişti
5s 7000mah yapık
2 6 s 60a esc oldu
</commit_message>
<xml_diff>
--- a/rapor dosyaları/Malzeme Talep ListesiV1 .xlsx
+++ b/rapor dosyaları/Malzeme Talep ListesiV1 .xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samet\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samet\OneDrive\Belgeler\GitHub\rapor dosyaları\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB9F9C8-649F-4F82-BBD9-249F841B186D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E21BC4-7789-45F1-82A5-8AC7C0147ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>leopard 4s 5200 mah batarya lipo</t>
   </si>
   <si>
-    <t>https://www.f1depo.com/urun/4s-5200mah-70c-lipo-batarya-14-8v-pil</t>
-  </si>
-  <si>
     <t>lora sx1276 868mhz iletişim modülü</t>
   </si>
   <si>
@@ -148,12 +145,6 @@
   </si>
   <si>
     <t>900kv motor</t>
-  </si>
-  <si>
-    <t>2s 4s  50a esc</t>
-  </si>
-  <si>
-    <t>https://www.robotistan.com/50-a-2s-4s-hobbywing-skywalker-esc-5v-5a-bec</t>
   </si>
   <si>
     <t>pixhawk px4 full set</t>
@@ -191,6 +182,15 @@
   </si>
   <si>
     <t>Konya Gıda ve Tarım Üniversitesi Kapsul Kongrul Takımı Malzeme Talep Listesi</t>
+  </si>
+  <si>
+    <t>2s 6s  60a esc 5v bec</t>
+  </si>
+  <si>
+    <t>https://www.promodelhobby.com/urun/emax-simon-series-60a-ubec-esc-2s-6s</t>
+  </si>
+  <si>
+    <t>https://www.f1depo.com/urun/5s-7000mah-40c-lipo-batarya-18-5v-pil</t>
   </si>
 </sst>
 </file>
@@ -433,8 +433,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -443,16 +453,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -672,7 +672,7 @@
   <dimension ref="A1:Y999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -688,13 +688,13 @@
   <sheetData>
     <row r="1" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -739,13 +739,13 @@
       <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>19</v>
+      <c r="B3" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="9">
         <v>3</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="11">
@@ -786,7 +786,7 @@
       <c r="C5" s="9">
         <v>3</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="11">
@@ -807,7 +807,7 @@
       <c r="C6" s="9">
         <v>14</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="12">
@@ -822,19 +822,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="9">
         <v>5</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>16</v>
+      <c r="D7" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="E7" s="12">
         <v>143.22999999999999</v>
       </c>
       <c r="F7" s="12">
-        <f>E7*C7</f>
+        <f t="shared" ref="F7:F16" si="1">E7*C7</f>
         <v>716.15</v>
       </c>
     </row>
@@ -843,19 +843,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="9">
         <v>10</v>
       </c>
-      <c r="D8" s="26" t="s">
-        <v>17</v>
+      <c r="D8" s="16" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="12">
         <v>225.98</v>
       </c>
       <c r="F8" s="12">
-        <f>E8*C8</f>
+        <f t="shared" si="1"/>
         <v>2259.7999999999997</v>
       </c>
     </row>
@@ -863,20 +863,20 @@
       <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>20</v>
+      <c r="B9" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="9">
         <v>10</v>
       </c>
-      <c r="D9" s="26" t="s">
-        <v>21</v>
+      <c r="D9" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="E9" s="12">
         <v>92</v>
       </c>
       <c r="F9" s="12">
-        <f>E9*C9</f>
+        <f t="shared" si="1"/>
         <v>920</v>
       </c>
     </row>
@@ -884,20 +884,20 @@
       <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>22</v>
+      <c r="B10" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="9">
         <v>2</v>
       </c>
-      <c r="D10" s="26" t="s">
-        <v>23</v>
+      <c r="D10" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="E10" s="12">
         <v>58.66</v>
       </c>
       <c r="F10" s="12">
-        <f>E10*C10</f>
+        <f t="shared" si="1"/>
         <v>117.32</v>
       </c>
     </row>
@@ -909,37 +909,37 @@
         <v>13</v>
       </c>
       <c r="C11" s="9">
-        <v>2</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="E11" s="12">
-        <v>1362</v>
+        <v>1770</v>
       </c>
       <c r="F11" s="12">
-        <f>E11*C11</f>
-        <v>2724</v>
+        <f t="shared" si="1"/>
+        <v>1770</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>25</v>
+      <c r="B12" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="9">
         <v>3</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>24</v>
+      <c r="D12" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="E12" s="12">
         <v>375</v>
       </c>
       <c r="F12" s="12">
-        <f>E12*C12</f>
+        <f t="shared" si="1"/>
         <v>1125</v>
       </c>
     </row>
@@ -947,41 +947,41 @@
       <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>26</v>
+      <c r="B13" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="C13" s="9">
         <v>2</v>
       </c>
-      <c r="D13" s="26" t="s">
-        <v>27</v>
+      <c r="D13" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="E13" s="12">
-        <v>308</v>
+        <v>448</v>
       </c>
       <c r="F13" s="12">
-        <f>E13*C13</f>
-        <v>616</v>
+        <f t="shared" si="1"/>
+        <v>896</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>12</v>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>28</v>
+      <c r="B14" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
       </c>
-      <c r="D14" s="26" t="s">
-        <v>29</v>
+      <c r="D14" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="E14" s="12">
         <v>4350</v>
       </c>
       <c r="F14" s="12">
-        <f>E14*C14</f>
+        <f t="shared" si="1"/>
         <v>4350</v>
       </c>
     </row>
@@ -989,20 +989,20 @@
       <c r="A15" s="7">
         <v>13</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>30</v>
+      <c r="B15" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>31</v>
+      <c r="D15" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="E15" s="12">
         <v>130</v>
       </c>
       <c r="F15" s="12">
-        <f>E15*C15</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
     </row>
@@ -1010,20 +1010,20 @@
       <c r="A16" s="7">
         <v>14</v>
       </c>
-      <c r="B16" s="29" t="s">
-        <v>32</v>
+      <c r="B16" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>33</v>
+      <c r="D16" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="E16" s="12">
         <v>404</v>
       </c>
       <c r="F16" s="12">
-        <f>E16*C16</f>
+        <f t="shared" si="1"/>
         <v>404</v>
       </c>
     </row>
@@ -1050,30 +1050,30 @@
       <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
+      <c r="A20" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="22"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="28"/>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -6952,10 +6952,10 @@
     <hyperlink ref="D9" r:id="rId7" display="https://tr.aliexpress.com/item/32637530520.html?srcSns=sns_Copy&amp;spreadType=socialShare&amp;bizType=ProductDetail&amp;social_params=60127423159&amp;aff_fcid=bf37b306aadd4171ab16a29eb2980848-1645624602972-08765-_uybzTN&amp;tt=MG&amp;aff_fsk=_uybzTN&amp;aff_platform=default&amp;sk=_uybzTN&amp;aff_trace_key=bf37b306aadd4171ab16a29eb2980848-1645624602972-08765-_uybzTN&amp;shareId=60127423159&amp;businessType=ProductDetail&amp;platform=AE&amp;terminal_id=bbdb96ebd8ef42e0996c8f6077033052&amp;afSmartRedirect=y" xr:uid="{92F5E79F-55A1-40D0-A89E-D2AD5CA2889B}"/>
     <hyperlink ref="D10" r:id="rId8" xr:uid="{55AEEE80-2C6E-4E53-ACE4-B6FCD979C937}"/>
     <hyperlink ref="D12" r:id="rId9" display="https://tr.aliexpress.com/item/1005001950159522.html?srcSns=sns_Copy&amp;spreadType=socialShare&amp;bizType=ProductDetail&amp;social_params=60141017997&amp;aff_fcid=cfd190b6eba34e66a47e07e0a7e333ef-1645625009909-00743-_voLUSG&amp;tt=MG&amp;aff_fsk=_voLUSG&amp;aff_platform=default&amp;sk=_voLUSG&amp;aff_trace_key=cfd190b6eba34e66a47e07e0a7e333ef-1645625009909-00743-_voLUSG&amp;shareId=60141017997&amp;businessType=ProductDetail&amp;platform=AE&amp;terminal_id=bbdb96ebd8ef42e0996c8f6077033052&amp;afSmartRedirect=y" xr:uid="{96A011A9-468C-40A7-94BF-9DE9F4BA957B}"/>
-    <hyperlink ref="D13" r:id="rId10" xr:uid="{5451E3F4-517D-49F8-A5DF-5D572EF093CA}"/>
-    <hyperlink ref="D14" r:id="rId11" xr:uid="{FDEFEF70-2E2B-41DF-A2DC-FC88B57FEA2D}"/>
-    <hyperlink ref="D16" r:id="rId12" xr:uid="{120B9B05-00C8-4508-99C0-65E9D1110D48}"/>
-    <hyperlink ref="D15" r:id="rId13" xr:uid="{A66262DB-2314-4FD2-9339-25A2D6ED1E15}"/>
+    <hyperlink ref="D14" r:id="rId10" xr:uid="{FDEFEF70-2E2B-41DF-A2DC-FC88B57FEA2D}"/>
+    <hyperlink ref="D16" r:id="rId11" xr:uid="{120B9B05-00C8-4508-99C0-65E9D1110D48}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{A66262DB-2314-4FD2-9339-25A2D6ED1E15}"/>
+    <hyperlink ref="D13" r:id="rId13" xr:uid="{118E338D-5220-4779-82DE-75BF16BAC928}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>

</xml_diff>

<commit_message>
esc 70 a oldu
</commit_message>
<xml_diff>
--- a/rapor dosyaları/Malzeme Talep ListesiV1 .xlsx
+++ b/rapor dosyaları/Malzeme Talep ListesiV1 .xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samet\OneDrive\Belgeler\GitHub\rapor dosyaları\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d82cb3954a51c9e/Belgeler/GitHub/rapor dosyaları/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E21BC4-7789-45F1-82A5-8AC7C0147ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{C8E21BC4-7789-45F1-82A5-8AC7C0147ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCFB8363-BB27-4487-8E9B-F2C2EA5AE302}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,13 +184,13 @@
     <t>Konya Gıda ve Tarım Üniversitesi Kapsul Kongrul Takımı Malzeme Talep Listesi</t>
   </si>
   <si>
-    <t>2s 6s  60a esc 5v bec</t>
+    <t>https://www.f1depo.com/urun/5s-7000mah-40c-lipo-batarya-18-5v-pil</t>
   </si>
   <si>
-    <t>https://www.promodelhobby.com/urun/emax-simon-series-60a-ubec-esc-2s-6s</t>
+    <t>https://www.promodelhobby.com/urun/ztw-beatles-70a-sbec-5-5v-3a-esc-2-6s</t>
   </si>
   <si>
-    <t>https://www.f1depo.com/urun/5s-7000mah-40c-lipo-batarya-18-5v-pil</t>
+    <t>2s 6s  70a esc 5v bec</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:Y999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -912,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="12">
         <v>1770</v>
@@ -948,7 +948,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" s="9">
         <v>2</v>
@@ -957,11 +957,11 @@
         <v>34</v>
       </c>
       <c r="E13" s="12">
-        <v>448</v>
+        <v>693</v>
       </c>
       <c r="F13" s="12">
         <f t="shared" si="1"/>
-        <v>896</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>